<commit_message>
Add Mainak Podder in Excel file
</commit_message>
<xml_diff>
--- a/Mainak.xlsx
+++ b/Mainak.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ALL\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBC6363-76FA-4E0F-A000-9F6F5BD78766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE59EE7-D3AB-4D77-ACA2-BB2C0CC22FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>a</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Mainak Podder</t>
   </si>
 </sst>
 </file>
@@ -351,15 +354,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,7 +376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -378,6 +384,9 @@
         <v>2</v>
       </c>
       <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>